<commit_message>
add functions for winning answers
</commit_message>
<xml_diff>
--- a/Questions to ask.xlsx
+++ b/Questions to ask.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>Hillz</t>
   </si>
@@ -117,6 +117,74 @@
   </si>
   <si>
     <t>a dog named Spinee???</t>
+  </si>
+  <si>
+    <t>announced their bid for presidency</t>
+  </si>
+  <si>
+    <t>67th United States Secretary of State</t>
+  </si>
+  <si>
+    <t>YouTube video</t>
+  </si>
+  <si>
+    <t xml:space="preserve">announced via </t>
+  </si>
+  <si>
+    <t>Hillary was in the 2015 Time magazine's "100 Most Influential People". Which of these people were also in that list?</t>
+  </si>
+  <si>
+    <t>Amy Schumer, Bradley Cooper, Kim Kardashian West, Ina Garten</t>
+  </si>
+  <si>
+    <t>Office</t>
+  </si>
+  <si>
+    <t>Clinton had taken a lease on a small office at 1 Pierrepont Plaza in Brooklyn, New York City -  Morgan Stanley has a major office in the building, which is also the home of the law office of Loretta E. Lynch</t>
+  </si>
+  <si>
+    <t>She stated that, "Everyday Americans need a champion. And I want to be that champion.</t>
+  </si>
+  <si>
+    <t>while Florida Senator Marco Rubio announced his candidacy on April 13, the day after Clinton. </t>
+  </si>
+  <si>
+    <t>Immediately following her announcement, she made a two-day road trip in a customized Chevrolet Express van, nicknamed after Scooby-Doo</t>
+  </si>
+  <si>
+    <t>Clinton held her first major campaign rally June 13, 2015, at Franklin D. Roosevelt Four Freedoms Park on the southern tip of New York City's Roosevelt Island.</t>
+  </si>
+  <si>
+    <t>Graphic designer Michael Bierut of the firm Pentagram designed the campaign's distinctive "H" logo;</t>
+  </si>
+  <si>
+    <t>Headquarters Brooklyn, New York, U.S.</t>
+  </si>
+  <si>
+    <t>Newsweek ranked her as the 13th most powerful person on the planet</t>
+  </si>
+  <si>
+    <t>In 2012, she was chosen as one of Barbara Walters' 10 Most Fascinating People of the year.[40]</t>
+  </si>
+  <si>
+    <t>Clinton has been ranked on their list of the world's most powerful people by Forbes magazine. She was listed as 5th most powerful in 2004,[67] 26th in 2005,[68] 18th in 2006,[69] 28th in 2008,[70] 36th in 2009,[71] 2nd in 2011,[72] 2nd in 2012,[73] 5th in 2013,[74] 6th in 2014, and 58th in 2015.[75][76]</t>
+  </si>
+  <si>
+    <t>Clinton has been named ten times in Time magazine's Time 100 as one of the 100 most influential people in the world.[77][78][79] Years this happened were 2004 (as part of The Clintons),[80] 2006,[81] 2007,[82] 2008,[83] 2009,[84] 2011,[85] 2012,[86] 2014,[77] 2015,[78] and 2016.[79] In addition, in November 2010, Time named Clinton one of the 25 most powerful women of the past century.[87]</t>
+  </si>
+  <si>
+    <t>Clinton has been named three times as Barbara Walters' Most Fascinating Person of the year, in 1993, 2003, and 2013.[88]</t>
+  </si>
+  <si>
+    <t>Family 
+Bill Clinton (Husband presidency) Chelsea Clinton (Daughter) Hugh E. Rodham (Father) Dorothy Howell Rodham (Mother) Hugh Rodham (Brother) Tony Rodham (Brother) Socks (Cat) Buddy (Dog) Whitehaven (house)</t>
+  </si>
+  <si>
+    <t>Writings 
+Bibliography Senior thesis (1969) It Takes a Village (1996) Dear Socks, Dear Buddy (1998) An Invitation to the White House (2000) Living History (2003) Hard Choices (2014)</t>
+  </si>
+  <si>
+    <t>Democratic blue to Republican red. A purple state refers to a swing state where both Democratic and Republican candidates receive strong support without an overwhelming majority of support for either party.</t>
   </si>
 </sst>
 </file>
@@ -152,9 +220,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -434,15 +505,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="105" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="49.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="45.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="66.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="74.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -455,7 +527,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -484,7 +556,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -495,7 +567,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -506,7 +578,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -514,7 +586,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -525,7 +597,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -533,7 +605,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -544,7 +616,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -554,20 +626,127 @@
         <v>23</v>
       </c>
     </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="2">
+        <v>42106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B23" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="B25" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="80" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="31" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="64" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="96" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="64" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="64" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add web images, css, and game logic
</commit_message>
<xml_diff>
--- a/Questions to ask.xlsx
+++ b/Questions to ask.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lynnfleck/src/Lynn-s-Project-1-Game/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lynnfleck/src/Pick-a-Pres/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>Hillz</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>Democratic blue to Republican red. A purple state refers to a swing state where both Democratic and Republican candidates receive strong support without an overwhelming majority of support for either party.</t>
+  </si>
+  <si>
+    <t>Trump's star on the Hollywood Walk of Fame</t>
+  </si>
+  <si>
+    <t>TIME "The 100 Most Influential People" (2016</t>
   </si>
 </sst>
 </file>
@@ -507,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="105" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -550,6 +556,11 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -683,15 +694,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="C33" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
@@ -699,47 +713,47 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="64" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="96" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="64" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="64" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
         <v>50</v>
       </c>

</xml_diff>